<commit_message>
Historial de cambios final
</commit_message>
<xml_diff>
--- a/src/gestorAplicacion/administrativo/historialDeCambios.xlsx
+++ b/src/gestorAplicacion/administrativo/historialDeCambios.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -429,17 +429,61 @@
       </c>
       <c r="B1" t="inlineStr">
         <is>
+          <t>Responsable</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
           <t>Nombre</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>Lote</t>
-        </is>
-      </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>Cantidad</t>
+          <t>Fecha</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Registro</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Asesor</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>32452</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>2025-02-06</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Pedido</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Asesor</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>asdsad</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>2025-02-06</t>
         </is>
       </c>
     </row>

</xml_diff>